<commit_message>
Creates valid eml and datasets that pass all congruency checks
</commit_message>
<xml_diff>
--- a/data-raw/mandy-salmanid-habitat-monitoring/Snorkel Index Data/snorkel-index-metadata.xlsx
+++ b/data-raw/mandy-salmanid-habitat-monitoring/Snorkel Index Data/snorkel-index-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abanet/Dropbox/B13/Data Files for Flow West/2020/Snorkel Index Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA_Salmonid_Habitat_Monitoring\data-raw\mandy-salmanid-habitat-monitoring\Snorkel Index Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1BE287-B6B4-7445-AB84-2D5D87CBFE64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED746933-7D7E-4511-AEA4-0CDF9CE95E63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12720" yWindow="800" windowWidth="24480" windowHeight="21140" tabRatio="834" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10080" yWindow="-16560" windowWidth="29040" windowHeight="15840" tabRatio="834" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="193">
   <si>
     <t>first_name</t>
   </si>
@@ -609,6 +609,12 @@
   </si>
   <si>
     <t>observer counted</t>
+  </si>
+  <si>
+    <t>wr_count</t>
+  </si>
+  <si>
+    <t>winter run counted</t>
   </si>
 </sst>
 </file>
@@ -616,7 +622,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -707,7 +713,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1099,12 +1105,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -1115,7 +1121,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -1144,16 +1150,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.625" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" customWidth="1"/>
-    <col min="10" max="10" width="32.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.375" customWidth="1"/>
+    <col min="10" max="10" width="32.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -1185,12 +1191,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -1208,32 +1214,32 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMH189"/>
+  <dimension ref="A1:AMH190"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="19.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.6640625" style="1"/>
-    <col min="3" max="3" width="13.1640625" style="10" customWidth="1"/>
+    <col min="1" max="2" width="19.625" style="1"/>
+    <col min="3" max="3" width="13.125" style="10" customWidth="1"/>
     <col min="4" max="4" width="17.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="13.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.125" style="10" customWidth="1"/>
     <col min="11" max="11" width="16" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1640625" style="1" customWidth="1"/>
-    <col min="15" max="1022" width="19.6640625" style="1"/>
-    <col min="1023" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="12" max="12" width="17.625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.125" style="1" customWidth="1"/>
+    <col min="15" max="1022" width="19.625" style="1"/>
+    <col min="1023" max="1025" width="8.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -1277,7 +1283,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>102</v>
       </c>
@@ -1309,7 +1315,7 @@
       </c>
       <c r="N2" s="15"/>
     </row>
-    <row r="3" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>165</v>
       </c>
@@ -1335,7 +1341,7 @@
       <c r="M3" s="13"/>
       <c r="N3" s="13"/>
     </row>
-    <row r="4" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>111</v>
       </c>
@@ -1361,7 +1367,7 @@
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>162</v>
       </c>
@@ -1399,7 +1405,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>113</v>
       </c>
@@ -1435,7 +1441,7 @@
         <v>3526</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>120</v>
       </c>
@@ -1461,7 +1467,7 @@
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
     </row>
-    <row r="8" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>123</v>
       </c>
@@ -1491,7 +1497,7 @@
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
     </row>
-    <row r="9" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>125</v>
       </c>
@@ -1527,7 +1533,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>128</v>
       </c>
@@ -1553,7 +1559,7 @@
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
     </row>
-    <row r="11" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>130</v>
       </c>
@@ -1589,7 +1595,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>134</v>
       </c>
@@ -1625,7 +1631,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>137</v>
       </c>
@@ -1661,7 +1667,7 @@
         <v>3.66</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>139</v>
       </c>
@@ -1687,7 +1693,7 @@
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
     </row>
-    <row r="15" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>141</v>
       </c>
@@ -1713,12 +1719,12 @@
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
     </row>
-    <row r="16" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>143</v>
+        <v>191</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>144</v>
+        <v>192</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>108</v>
@@ -1749,12 +1755,12 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>108</v>
@@ -1785,12 +1791,12 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>108</v>
@@ -1821,12 +1827,12 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>108</v>
@@ -1857,12 +1863,12 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>108</v>
@@ -1893,12 +1899,12 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>108</v>
@@ -1929,85 +1935,105 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
+        <v>132</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>146</v>
+      </c>
       <c r="J22" s="14"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-    </row>
-    <row r="23" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="M22" s="13">
+        <v>0</v>
+      </c>
+      <c r="N22" s="13">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>127</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
       <c r="J23" s="14"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
-      <c r="M23" s="13">
-        <v>0</v>
-      </c>
-      <c r="N23" s="13">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+    </row>
+    <row r="24" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>117</v>
+      </c>
       <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
+      <c r="F24" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>127</v>
+      </c>
       <c r="J24" s="14"/>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M24" s="13">
+        <v>0</v>
+      </c>
+      <c r="N24" s="13">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="14"/>
@@ -2023,7 +2049,7 @@
       <c r="M25" s="13"/>
       <c r="N25" s="13"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="14"/>
@@ -2039,7 +2065,7 @@
       <c r="M26" s="13"/>
       <c r="N26" s="13"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="14"/>
@@ -2055,7 +2081,7 @@
       <c r="M27" s="13"/>
       <c r="N27" s="13"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="14"/>
@@ -2071,7 +2097,7 @@
       <c r="M28" s="13"/>
       <c r="N28" s="13"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="14"/>
@@ -2087,7 +2113,7 @@
       <c r="M29" s="13"/>
       <c r="N29" s="13"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="14"/>
@@ -2103,7 +2129,7 @@
       <c r="M30" s="13"/>
       <c r="N30" s="13"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="14"/>
@@ -2119,7 +2145,7 @@
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="14"/>
@@ -2135,7 +2161,7 @@
       <c r="M32" s="13"/>
       <c r="N32" s="13"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="14"/>
@@ -2151,7 +2177,7 @@
       <c r="M33" s="13"/>
       <c r="N33" s="13"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="14"/>
@@ -2167,7 +2193,7 @@
       <c r="M34" s="13"/>
       <c r="N34" s="13"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="14"/>
@@ -2183,7 +2209,7 @@
       <c r="M35" s="13"/>
       <c r="N35" s="13"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="14"/>
@@ -2199,7 +2225,7 @@
       <c r="M36" s="13"/>
       <c r="N36" s="13"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="14"/>
@@ -2215,7 +2241,7 @@
       <c r="M37" s="13"/>
       <c r="N37" s="13"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="14"/>
@@ -2231,7 +2257,7 @@
       <c r="M38" s="13"/>
       <c r="N38" s="13"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="14"/>
@@ -2247,7 +2273,7 @@
       <c r="M39" s="13"/>
       <c r="N39" s="13"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="14"/>
@@ -2263,7 +2289,7 @@
       <c r="M40" s="13"/>
       <c r="N40" s="13"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="14"/>
@@ -2279,7 +2305,7 @@
       <c r="M41" s="13"/>
       <c r="N41" s="13"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="14"/>
@@ -2295,7 +2321,7 @@
       <c r="M42" s="13"/>
       <c r="N42" s="13"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="14"/>
@@ -2311,7 +2337,7 @@
       <c r="M43" s="13"/>
       <c r="N43" s="13"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="14"/>
@@ -2327,7 +2353,7 @@
       <c r="M44" s="13"/>
       <c r="N44" s="13"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="14"/>
@@ -2343,7 +2369,7 @@
       <c r="M45" s="13"/>
       <c r="N45" s="13"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="14"/>
@@ -2359,7 +2385,7 @@
       <c r="M46" s="13"/>
       <c r="N46" s="13"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="14"/>
@@ -2375,7 +2401,7 @@
       <c r="M47" s="13"/>
       <c r="N47" s="13"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="14"/>
@@ -2391,7 +2417,7 @@
       <c r="M48" s="13"/>
       <c r="N48" s="13"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="14"/>
@@ -2407,7 +2433,7 @@
       <c r="M49" s="13"/>
       <c r="N49" s="13"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="14"/>
@@ -2423,7 +2449,7 @@
       <c r="M50" s="13"/>
       <c r="N50" s="13"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="14"/>
@@ -2439,7 +2465,7 @@
       <c r="M51" s="13"/>
       <c r="N51" s="13"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="14"/>
@@ -2455,7 +2481,7 @@
       <c r="M52" s="13"/>
       <c r="N52" s="13"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="14"/>
@@ -2471,7 +2497,7 @@
       <c r="M53" s="13"/>
       <c r="N53" s="13"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="14"/>
@@ -2487,7 +2513,7 @@
       <c r="M54" s="13"/>
       <c r="N54" s="13"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="14"/>
@@ -2503,7 +2529,7 @@
       <c r="M55" s="13"/>
       <c r="N55" s="13"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="14"/>
@@ -2519,7 +2545,7 @@
       <c r="M56" s="13"/>
       <c r="N56" s="13"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="14"/>
@@ -2535,7 +2561,7 @@
       <c r="M57" s="13"/>
       <c r="N57" s="13"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="14"/>
@@ -2551,7 +2577,7 @@
       <c r="M58" s="13"/>
       <c r="N58" s="13"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="14"/>
@@ -2567,7 +2593,7 @@
       <c r="M59" s="13"/>
       <c r="N59" s="13"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="14"/>
@@ -2583,7 +2609,7 @@
       <c r="M60" s="13"/>
       <c r="N60" s="13"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="C61" s="14"/>
@@ -2599,7 +2625,7 @@
       <c r="M61" s="13"/>
       <c r="N61" s="13"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="14"/>
@@ -2615,7 +2641,7 @@
       <c r="M62" s="13"/>
       <c r="N62" s="13"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="14"/>
@@ -2631,7 +2657,7 @@
       <c r="M63" s="13"/>
       <c r="N63" s="13"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="14"/>
@@ -2647,7 +2673,7 @@
       <c r="M64" s="13"/>
       <c r="N64" s="13"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="14"/>
@@ -2663,7 +2689,7 @@
       <c r="M65" s="13"/>
       <c r="N65" s="13"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
       <c r="C66" s="14"/>
@@ -2679,7 +2705,7 @@
       <c r="M66" s="13"/>
       <c r="N66" s="13"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="14"/>
@@ -2695,7 +2721,7 @@
       <c r="M67" s="13"/>
       <c r="N67" s="13"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="C68" s="14"/>
@@ -2711,7 +2737,7 @@
       <c r="M68" s="13"/>
       <c r="N68" s="13"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="C69" s="14"/>
@@ -2727,7 +2753,7 @@
       <c r="M69" s="13"/>
       <c r="N69" s="13"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="C70" s="14"/>
@@ -2743,7 +2769,7 @@
       <c r="M70" s="13"/>
       <c r="N70" s="13"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="C71" s="14"/>
@@ -2759,7 +2785,7 @@
       <c r="M71" s="13"/>
       <c r="N71" s="13"/>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="14"/>
@@ -2775,7 +2801,7 @@
       <c r="M72" s="13"/>
       <c r="N72" s="13"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="14"/>
@@ -2791,7 +2817,7 @@
       <c r="M73" s="13"/>
       <c r="N73" s="13"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="14"/>
@@ -2807,7 +2833,7 @@
       <c r="M74" s="13"/>
       <c r="N74" s="13"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="14"/>
@@ -2823,7 +2849,7 @@
       <c r="M75" s="13"/>
       <c r="N75" s="13"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="14"/>
@@ -2839,7 +2865,7 @@
       <c r="M76" s="13"/>
       <c r="N76" s="13"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="13"/>
       <c r="B77" s="13"/>
       <c r="C77" s="14"/>
@@ -2855,7 +2881,7 @@
       <c r="M77" s="13"/>
       <c r="N77" s="13"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
       <c r="B78" s="13"/>
       <c r="C78" s="14"/>
@@ -2871,7 +2897,7 @@
       <c r="M78" s="13"/>
       <c r="N78" s="13"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="13"/>
       <c r="B79" s="13"/>
       <c r="C79" s="14"/>
@@ -2887,7 +2913,7 @@
       <c r="M79" s="13"/>
       <c r="N79" s="13"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="13"/>
       <c r="B80" s="13"/>
       <c r="C80" s="14"/>
@@ -2903,7 +2929,7 @@
       <c r="M80" s="13"/>
       <c r="N80" s="13"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="13"/>
       <c r="B81" s="13"/>
       <c r="C81" s="14"/>
@@ -2919,7 +2945,7 @@
       <c r="M81" s="13"/>
       <c r="N81" s="13"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="13"/>
       <c r="B82" s="13"/>
       <c r="C82" s="14"/>
@@ -2935,7 +2961,7 @@
       <c r="M82" s="13"/>
       <c r="N82" s="13"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="13"/>
       <c r="B83" s="13"/>
       <c r="C83" s="14"/>
@@ -2951,7 +2977,7 @@
       <c r="M83" s="13"/>
       <c r="N83" s="13"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="13"/>
       <c r="B84" s="13"/>
       <c r="C84" s="14"/>
@@ -2967,7 +2993,7 @@
       <c r="M84" s="13"/>
       <c r="N84" s="13"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="C85" s="14"/>
@@ -2983,7 +3009,7 @@
       <c r="M85" s="13"/>
       <c r="N85" s="13"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="13"/>
       <c r="B86" s="13"/>
       <c r="C86" s="14"/>
@@ -2999,7 +3025,7 @@
       <c r="M86" s="13"/>
       <c r="N86" s="13"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="13"/>
       <c r="B87" s="13"/>
       <c r="C87" s="14"/>
@@ -3015,7 +3041,7 @@
       <c r="M87" s="13"/>
       <c r="N87" s="13"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="13"/>
       <c r="B88" s="13"/>
       <c r="C88" s="14"/>
@@ -3031,7 +3057,7 @@
       <c r="M88" s="13"/>
       <c r="N88" s="13"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="13"/>
       <c r="B89" s="13"/>
       <c r="C89" s="14"/>
@@ -3047,7 +3073,7 @@
       <c r="M89" s="13"/>
       <c r="N89" s="13"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="13"/>
       <c r="B90" s="13"/>
       <c r="C90" s="14"/>
@@ -3063,7 +3089,7 @@
       <c r="M90" s="13"/>
       <c r="N90" s="13"/>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
       <c r="C91" s="14"/>
@@ -3079,7 +3105,7 @@
       <c r="M91" s="13"/>
       <c r="N91" s="13"/>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="13"/>
       <c r="B92" s="13"/>
       <c r="C92" s="14"/>
@@ -3095,7 +3121,7 @@
       <c r="M92" s="13"/>
       <c r="N92" s="13"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
       <c r="B93" s="13"/>
       <c r="C93" s="14"/>
@@ -3111,7 +3137,7 @@
       <c r="M93" s="13"/>
       <c r="N93" s="13"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
       <c r="B94" s="13"/>
       <c r="C94" s="14"/>
@@ -3127,7 +3153,7 @@
       <c r="M94" s="13"/>
       <c r="N94" s="13"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="13"/>
       <c r="B95" s="13"/>
       <c r="C95" s="14"/>
@@ -3143,7 +3169,7 @@
       <c r="M95" s="13"/>
       <c r="N95" s="13"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="13"/>
       <c r="B96" s="13"/>
       <c r="C96" s="14"/>
@@ -3159,7 +3185,7 @@
       <c r="M96" s="13"/>
       <c r="N96" s="13"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>
       <c r="B97" s="13"/>
       <c r="C97" s="14"/>
@@ -3175,7 +3201,7 @@
       <c r="M97" s="13"/>
       <c r="N97" s="13"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="13"/>
       <c r="B98" s="13"/>
       <c r="C98" s="14"/>
@@ -3191,7 +3217,7 @@
       <c r="M98" s="13"/>
       <c r="N98" s="13"/>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="13"/>
       <c r="B99" s="13"/>
       <c r="C99" s="14"/>
@@ -3207,7 +3233,7 @@
       <c r="M99" s="13"/>
       <c r="N99" s="13"/>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="13"/>
       <c r="B100" s="13"/>
       <c r="C100" s="14"/>
@@ -3223,7 +3249,7 @@
       <c r="M100" s="13"/>
       <c r="N100" s="13"/>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
       <c r="B101" s="13"/>
       <c r="C101" s="14"/>
@@ -3239,7 +3265,7 @@
       <c r="M101" s="13"/>
       <c r="N101" s="13"/>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="13"/>
       <c r="B102" s="13"/>
       <c r="C102" s="14"/>
@@ -3255,7 +3281,7 @@
       <c r="M102" s="13"/>
       <c r="N102" s="13"/>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="13"/>
       <c r="B103" s="13"/>
       <c r="C103" s="14"/>
@@ -3271,7 +3297,7 @@
       <c r="M103" s="13"/>
       <c r="N103" s="13"/>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="13"/>
       <c r="B104" s="13"/>
       <c r="C104" s="14"/>
@@ -3287,7 +3313,7 @@
       <c r="M104" s="13"/>
       <c r="N104" s="13"/>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="13"/>
       <c r="B105" s="13"/>
       <c r="C105" s="14"/>
@@ -3303,7 +3329,7 @@
       <c r="M105" s="13"/>
       <c r="N105" s="13"/>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="13"/>
       <c r="B106" s="13"/>
       <c r="C106" s="14"/>
@@ -3319,7 +3345,7 @@
       <c r="M106" s="13"/>
       <c r="N106" s="13"/>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="13"/>
       <c r="B107" s="13"/>
       <c r="C107" s="14"/>
@@ -3335,7 +3361,7 @@
       <c r="M107" s="13"/>
       <c r="N107" s="13"/>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="13"/>
       <c r="B108" s="13"/>
       <c r="C108" s="14"/>
@@ -3351,7 +3377,7 @@
       <c r="M108" s="13"/>
       <c r="N108" s="13"/>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="13"/>
       <c r="B109" s="13"/>
       <c r="C109" s="14"/>
@@ -3367,7 +3393,7 @@
       <c r="M109" s="13"/>
       <c r="N109" s="13"/>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="13"/>
       <c r="B110" s="13"/>
       <c r="C110" s="14"/>
@@ -3383,7 +3409,7 @@
       <c r="M110" s="13"/>
       <c r="N110" s="13"/>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="13"/>
       <c r="B111" s="13"/>
       <c r="C111" s="14"/>
@@ -3399,7 +3425,7 @@
       <c r="M111" s="13"/>
       <c r="N111" s="13"/>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="13"/>
       <c r="B112" s="13"/>
       <c r="C112" s="14"/>
@@ -3415,7 +3441,7 @@
       <c r="M112" s="13"/>
       <c r="N112" s="13"/>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" s="13"/>
       <c r="B113" s="13"/>
       <c r="C113" s="14"/>
@@ -3431,7 +3457,7 @@
       <c r="M113" s="13"/>
       <c r="N113" s="13"/>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="13"/>
       <c r="B114" s="13"/>
       <c r="C114" s="14"/>
@@ -3447,7 +3473,7 @@
       <c r="M114" s="13"/>
       <c r="N114" s="13"/>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="13"/>
       <c r="B115" s="13"/>
       <c r="C115" s="14"/>
@@ -3463,7 +3489,7 @@
       <c r="M115" s="13"/>
       <c r="N115" s="13"/>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="13"/>
       <c r="B116" s="13"/>
       <c r="C116" s="14"/>
@@ -3479,7 +3505,7 @@
       <c r="M116" s="13"/>
       <c r="N116" s="13"/>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
       <c r="B117" s="13"/>
       <c r="C117" s="14"/>
@@ -3495,7 +3521,7 @@
       <c r="M117" s="13"/>
       <c r="N117" s="13"/>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" s="13"/>
       <c r="B118" s="13"/>
       <c r="C118" s="14"/>
@@ -3511,7 +3537,7 @@
       <c r="M118" s="13"/>
       <c r="N118" s="13"/>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="13"/>
       <c r="B119" s="13"/>
       <c r="C119" s="14"/>
@@ -3527,7 +3553,7 @@
       <c r="M119" s="13"/>
       <c r="N119" s="13"/>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" s="13"/>
       <c r="B120" s="13"/>
       <c r="C120" s="14"/>
@@ -3543,7 +3569,7 @@
       <c r="M120" s="13"/>
       <c r="N120" s="13"/>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" s="13"/>
       <c r="B121" s="13"/>
       <c r="C121" s="14"/>
@@ -3559,7 +3585,7 @@
       <c r="M121" s="13"/>
       <c r="N121" s="13"/>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" s="13"/>
       <c r="B122" s="13"/>
       <c r="C122" s="14"/>
@@ -3575,7 +3601,7 @@
       <c r="M122" s="13"/>
       <c r="N122" s="13"/>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" s="13"/>
       <c r="B123" s="13"/>
       <c r="C123" s="14"/>
@@ -3591,7 +3617,7 @@
       <c r="M123" s="13"/>
       <c r="N123" s="13"/>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" s="13"/>
       <c r="B124" s="13"/>
       <c r="C124" s="14"/>
@@ -3607,7 +3633,7 @@
       <c r="M124" s="13"/>
       <c r="N124" s="13"/>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" s="13"/>
       <c r="B125" s="13"/>
       <c r="C125" s="14"/>
@@ -3623,7 +3649,7 @@
       <c r="M125" s="13"/>
       <c r="N125" s="13"/>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" s="13"/>
       <c r="B126" s="13"/>
       <c r="C126" s="14"/>
@@ -3639,7 +3665,7 @@
       <c r="M126" s="13"/>
       <c r="N126" s="13"/>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" s="13"/>
       <c r="B127" s="13"/>
       <c r="C127" s="14"/>
@@ -3655,7 +3681,7 @@
       <c r="M127" s="13"/>
       <c r="N127" s="13"/>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" s="13"/>
       <c r="B128" s="13"/>
       <c r="C128" s="14"/>
@@ -3671,7 +3697,7 @@
       <c r="M128" s="13"/>
       <c r="N128" s="13"/>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" s="13"/>
       <c r="B129" s="13"/>
       <c r="C129" s="14"/>
@@ -3687,7 +3713,7 @@
       <c r="M129" s="13"/>
       <c r="N129" s="13"/>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" s="13"/>
       <c r="B130" s="13"/>
       <c r="C130" s="14"/>
@@ -3703,7 +3729,7 @@
       <c r="M130" s="13"/>
       <c r="N130" s="13"/>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" s="13"/>
       <c r="B131" s="13"/>
       <c r="C131" s="14"/>
@@ -3719,7 +3745,7 @@
       <c r="M131" s="13"/>
       <c r="N131" s="13"/>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" s="13"/>
       <c r="B132" s="13"/>
       <c r="C132" s="14"/>
@@ -3735,7 +3761,7 @@
       <c r="M132" s="13"/>
       <c r="N132" s="13"/>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="13"/>
       <c r="B133" s="13"/>
       <c r="C133" s="14"/>
@@ -3751,7 +3777,7 @@
       <c r="M133" s="13"/>
       <c r="N133" s="13"/>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" s="13"/>
       <c r="B134" s="13"/>
       <c r="C134" s="14"/>
@@ -3767,7 +3793,7 @@
       <c r="M134" s="13"/>
       <c r="N134" s="13"/>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="13"/>
       <c r="B135" s="13"/>
       <c r="C135" s="14"/>
@@ -3783,7 +3809,7 @@
       <c r="M135" s="13"/>
       <c r="N135" s="13"/>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="13"/>
       <c r="B136" s="13"/>
       <c r="C136" s="14"/>
@@ -3799,7 +3825,7 @@
       <c r="M136" s="13"/>
       <c r="N136" s="13"/>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="13"/>
       <c r="B137" s="13"/>
       <c r="C137" s="14"/>
@@ -3815,7 +3841,7 @@
       <c r="M137" s="13"/>
       <c r="N137" s="13"/>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" s="13"/>
       <c r="B138" s="13"/>
       <c r="C138" s="14"/>
@@ -3831,7 +3857,7 @@
       <c r="M138" s="13"/>
       <c r="N138" s="13"/>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" s="13"/>
       <c r="B139" s="13"/>
       <c r="C139" s="14"/>
@@ -3847,7 +3873,7 @@
       <c r="M139" s="13"/>
       <c r="N139" s="13"/>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" s="13"/>
       <c r="B140" s="13"/>
       <c r="C140" s="14"/>
@@ -3863,7 +3889,7 @@
       <c r="M140" s="13"/>
       <c r="N140" s="13"/>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" s="13"/>
       <c r="B141" s="13"/>
       <c r="C141" s="14"/>
@@ -3879,7 +3905,7 @@
       <c r="M141" s="13"/>
       <c r="N141" s="13"/>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" s="13"/>
       <c r="B142" s="13"/>
       <c r="C142" s="14"/>
@@ -3895,7 +3921,7 @@
       <c r="M142" s="13"/>
       <c r="N142" s="13"/>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" s="13"/>
       <c r="B143" s="13"/>
       <c r="C143" s="14"/>
@@ -3911,7 +3937,7 @@
       <c r="M143" s="13"/>
       <c r="N143" s="13"/>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" s="13"/>
       <c r="B144" s="13"/>
       <c r="C144" s="14"/>
@@ -3927,7 +3953,7 @@
       <c r="M144" s="13"/>
       <c r="N144" s="13"/>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" s="13"/>
       <c r="B145" s="13"/>
       <c r="C145" s="14"/>
@@ -3943,7 +3969,7 @@
       <c r="M145" s="13"/>
       <c r="N145" s="13"/>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" s="13"/>
       <c r="B146" s="13"/>
       <c r="C146" s="14"/>
@@ -3959,7 +3985,7 @@
       <c r="M146" s="13"/>
       <c r="N146" s="13"/>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" s="13"/>
       <c r="B147" s="13"/>
       <c r="C147" s="14"/>
@@ -3975,7 +4001,7 @@
       <c r="M147" s="13"/>
       <c r="N147" s="13"/>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" s="13"/>
       <c r="B148" s="13"/>
       <c r="C148" s="14"/>
@@ -3991,7 +4017,7 @@
       <c r="M148" s="13"/>
       <c r="N148" s="13"/>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" s="13"/>
       <c r="B149" s="13"/>
       <c r="C149" s="14"/>
@@ -4007,7 +4033,7 @@
       <c r="M149" s="13"/>
       <c r="N149" s="13"/>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" s="13"/>
       <c r="B150" s="13"/>
       <c r="C150" s="14"/>
@@ -4023,7 +4049,7 @@
       <c r="M150" s="13"/>
       <c r="N150" s="13"/>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" s="13"/>
       <c r="B151" s="13"/>
       <c r="C151" s="14"/>
@@ -4039,7 +4065,7 @@
       <c r="M151" s="13"/>
       <c r="N151" s="13"/>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" s="13"/>
       <c r="B152" s="13"/>
       <c r="C152" s="14"/>
@@ -4055,7 +4081,7 @@
       <c r="M152" s="13"/>
       <c r="N152" s="13"/>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" s="13"/>
       <c r="B153" s="13"/>
       <c r="C153" s="14"/>
@@ -4071,7 +4097,7 @@
       <c r="M153" s="13"/>
       <c r="N153" s="13"/>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" s="13"/>
       <c r="B154" s="13"/>
       <c r="C154" s="14"/>
@@ -4087,7 +4113,7 @@
       <c r="M154" s="13"/>
       <c r="N154" s="13"/>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" s="13"/>
       <c r="B155" s="13"/>
       <c r="C155" s="14"/>
@@ -4103,7 +4129,7 @@
       <c r="M155" s="13"/>
       <c r="N155" s="13"/>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" s="13"/>
       <c r="B156" s="13"/>
       <c r="C156" s="14"/>
@@ -4119,7 +4145,7 @@
       <c r="M156" s="13"/>
       <c r="N156" s="13"/>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157" s="13"/>
       <c r="B157" s="13"/>
       <c r="C157" s="14"/>
@@ -4135,7 +4161,7 @@
       <c r="M157" s="13"/>
       <c r="N157" s="13"/>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" s="13"/>
       <c r="B158" s="13"/>
       <c r="C158" s="14"/>
@@ -4151,7 +4177,7 @@
       <c r="M158" s="13"/>
       <c r="N158" s="13"/>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159" s="13"/>
       <c r="B159" s="13"/>
       <c r="C159" s="14"/>
@@ -4167,7 +4193,7 @@
       <c r="M159" s="13"/>
       <c r="N159" s="13"/>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" s="13"/>
       <c r="B160" s="13"/>
       <c r="C160" s="14"/>
@@ -4183,7 +4209,7 @@
       <c r="M160" s="13"/>
       <c r="N160" s="13"/>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" s="13"/>
       <c r="B161" s="13"/>
       <c r="C161" s="14"/>
@@ -4199,7 +4225,7 @@
       <c r="M161" s="13"/>
       <c r="N161" s="13"/>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" s="13"/>
       <c r="B162" s="13"/>
       <c r="C162" s="14"/>
@@ -4215,7 +4241,7 @@
       <c r="M162" s="13"/>
       <c r="N162" s="13"/>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" s="13"/>
       <c r="B163" s="13"/>
       <c r="C163" s="14"/>
@@ -4231,7 +4257,7 @@
       <c r="M163" s="13"/>
       <c r="N163" s="13"/>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" s="13"/>
       <c r="B164" s="13"/>
       <c r="C164" s="14"/>
@@ -4247,7 +4273,7 @@
       <c r="M164" s="13"/>
       <c r="N164" s="13"/>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" s="13"/>
       <c r="B165" s="13"/>
       <c r="C165" s="14"/>
@@ -4263,7 +4289,7 @@
       <c r="M165" s="13"/>
       <c r="N165" s="13"/>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" s="13"/>
       <c r="B166" s="13"/>
       <c r="C166" s="14"/>
@@ -4279,7 +4305,7 @@
       <c r="M166" s="13"/>
       <c r="N166" s="13"/>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" s="13"/>
       <c r="B167" s="13"/>
       <c r="C167" s="14"/>
@@ -4295,7 +4321,7 @@
       <c r="M167" s="13"/>
       <c r="N167" s="13"/>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A168" s="13"/>
       <c r="B168" s="13"/>
       <c r="C168" s="14"/>
@@ -4311,7 +4337,7 @@
       <c r="M168" s="13"/>
       <c r="N168" s="13"/>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A169" s="13"/>
       <c r="B169" s="13"/>
       <c r="C169" s="14"/>
@@ -4327,7 +4353,7 @@
       <c r="M169" s="13"/>
       <c r="N169" s="13"/>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A170" s="13"/>
       <c r="B170" s="13"/>
       <c r="C170" s="14"/>
@@ -4343,7 +4369,7 @@
       <c r="M170" s="13"/>
       <c r="N170" s="13"/>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A171" s="13"/>
       <c r="B171" s="13"/>
       <c r="C171" s="14"/>
@@ -4359,7 +4385,7 @@
       <c r="M171" s="13"/>
       <c r="N171" s="13"/>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A172" s="13"/>
       <c r="B172" s="13"/>
       <c r="C172" s="14"/>
@@ -4375,7 +4401,7 @@
       <c r="M172" s="13"/>
       <c r="N172" s="13"/>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" s="13"/>
       <c r="B173" s="13"/>
       <c r="C173" s="14"/>
@@ -4391,7 +4417,7 @@
       <c r="M173" s="13"/>
       <c r="N173" s="13"/>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" s="13"/>
       <c r="B174" s="13"/>
       <c r="C174" s="14"/>
@@ -4407,7 +4433,7 @@
       <c r="M174" s="13"/>
       <c r="N174" s="13"/>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" s="13"/>
       <c r="B175" s="13"/>
       <c r="C175" s="14"/>
@@ -4423,7 +4449,7 @@
       <c r="M175" s="13"/>
       <c r="N175" s="13"/>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" s="13"/>
       <c r="B176" s="13"/>
       <c r="C176" s="14"/>
@@ -4439,7 +4465,7 @@
       <c r="M176" s="13"/>
       <c r="N176" s="13"/>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A177" s="13"/>
       <c r="B177" s="13"/>
       <c r="C177" s="14"/>
@@ -4455,7 +4481,7 @@
       <c r="M177" s="13"/>
       <c r="N177" s="13"/>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A178" s="13"/>
       <c r="B178" s="13"/>
       <c r="C178" s="14"/>
@@ -4471,7 +4497,7 @@
       <c r="M178" s="13"/>
       <c r="N178" s="13"/>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A179" s="13"/>
       <c r="B179" s="13"/>
       <c r="C179" s="14"/>
@@ -4487,7 +4513,7 @@
       <c r="M179" s="13"/>
       <c r="N179" s="13"/>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A180" s="13"/>
       <c r="B180" s="13"/>
       <c r="C180" s="14"/>
@@ -4503,7 +4529,7 @@
       <c r="M180" s="13"/>
       <c r="N180" s="13"/>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A181" s="13"/>
       <c r="B181" s="13"/>
       <c r="C181" s="14"/>
@@ -4519,7 +4545,7 @@
       <c r="M181" s="13"/>
       <c r="N181" s="13"/>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A182" s="13"/>
       <c r="B182" s="13"/>
       <c r="C182" s="14"/>
@@ -4535,7 +4561,7 @@
       <c r="M182" s="13"/>
       <c r="N182" s="13"/>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A183" s="13"/>
       <c r="B183" s="13"/>
       <c r="C183" s="14"/>
@@ -4551,7 +4577,7 @@
       <c r="M183" s="13"/>
       <c r="N183" s="13"/>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A184" s="13"/>
       <c r="B184" s="13"/>
       <c r="C184" s="14"/>
@@ -4567,7 +4593,7 @@
       <c r="M184" s="13"/>
       <c r="N184" s="13"/>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A185" s="13"/>
       <c r="B185" s="13"/>
       <c r="C185" s="14"/>
@@ -4583,7 +4609,7 @@
       <c r="M185" s="13"/>
       <c r="N185" s="13"/>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A186" s="13"/>
       <c r="B186" s="13"/>
       <c r="C186" s="14"/>
@@ -4599,7 +4625,7 @@
       <c r="M186" s="13"/>
       <c r="N186" s="13"/>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A187" s="13"/>
       <c r="B187" s="13"/>
       <c r="C187" s="14"/>
@@ -4615,7 +4641,7 @@
       <c r="M187" s="13"/>
       <c r="N187" s="13"/>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A188" s="13"/>
       <c r="B188" s="13"/>
       <c r="C188" s="14"/>
@@ -4631,7 +4657,7 @@
       <c r="M188" s="13"/>
       <c r="N188" s="13"/>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A189" s="13"/>
       <c r="B189" s="13"/>
       <c r="C189" s="14"/>
@@ -4647,29 +4673,45 @@
       <c r="M189" s="13"/>
       <c r="N189" s="13"/>
     </row>
+    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A190" s="13"/>
+      <c r="B190" s="13"/>
+      <c r="C190" s="14"/>
+      <c r="D190" s="13"/>
+      <c r="E190" s="13"/>
+      <c r="F190" s="13"/>
+      <c r="G190" s="13"/>
+      <c r="H190" s="13"/>
+      <c r="I190" s="13"/>
+      <c r="J190" s="14"/>
+      <c r="K190" s="13"/>
+      <c r="L190" s="13"/>
+      <c r="M190" s="13"/>
+      <c r="N190" s="13"/>
+    </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1022" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F11 F13:F1023" xr:uid="{00000000-0002-0000-0800-000001000000}">
+      <formula1>"text,enumerated,dateTime,numeric"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1 I191:I1023" xr:uid="{00000000-0002-0000-0800-000002000000}">
+      <formula1>"natural,whole,interger,real"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G11 G13:G1023" xr:uid="{00000000-0002-0000-0800-000003000000}">
+      <formula1>"ratio,interval"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{483D7C4D-3CB6-404A-B9C1-693F9BA7B223}">
+      <formula1>M2</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1023" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F11 F13:F1022" xr:uid="{00000000-0002-0000-0800-000001000000}">
-      <formula1>"text,enumerated,dateTime,numeric"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1 I190:I1022" xr:uid="{00000000-0002-0000-0800-000002000000}">
-      <formula1>"natural,whole,interger,real"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G11 G13:G1022" xr:uid="{00000000-0002-0000-0800-000003000000}">
-      <formula1>"ratio,interval"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I189" xr:uid="{80B4E72A-B887-DF48-89F3-3DAE24F60A4C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I190" xr:uid="{80B4E72A-B887-DF48-89F3-3DAE24F60A4C}">
       <formula1>"whole, real, integer, natural"</formula1>
-    </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{483D7C4D-3CB6-404A-B9C1-693F9BA7B223}">
-      <formula1>M2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4685,14 +4727,14 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -4703,7 +4745,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4714,7 +4756,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4725,7 +4767,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4736,7 +4778,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4747,7 +4789,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4758,7 +4800,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4769,7 +4811,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>175</v>
       </c>
@@ -4780,7 +4822,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>177</v>
       </c>
@@ -4791,7 +4833,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>179</v>
       </c>
@@ -4802,7 +4844,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>181</v>
       </c>
@@ -4813,7 +4855,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>182</v>
       </c>
@@ -4824,7 +4866,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>183</v>
       </c>
@@ -4835,7 +4877,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>184</v>
       </c>
@@ -4846,7 +4888,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>185</v>
       </c>
@@ -4857,7 +4899,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>187</v>
       </c>
@@ -4868,7 +4910,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>189</v>
       </c>
@@ -4893,15 +4935,15 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="25.625" customWidth="1"/>
+    <col min="5" max="5" width="27.375" customWidth="1"/>
     <col min="6" max="6" width="27" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4921,7 +4963,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -4941,7 +4983,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -4961,7 +5003,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -4978,7 +5020,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -5022,13 +5064,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="34.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -5036,7 +5078,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="115" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>89</v>
       </c>
@@ -5058,13 +5100,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="46.625" customWidth="1"/>
+    <col min="2" max="2" width="22.375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -5072,22 +5114,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -5106,15 +5148,15 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.375" customWidth="1"/>
+    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5131,7 +5173,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -5155,18 +5197,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="38.125" customWidth="1"/>
+    <col min="2" max="2" width="12.375" customWidth="1"/>
+    <col min="3" max="3" width="13.125" customWidth="1"/>
+    <col min="4" max="4" width="17.875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.875" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
     <col min="7" max="7" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5189,7 +5231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -5234,17 +5276,17 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="21.625" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="7"/>
-    <col min="6" max="6" width="17.33203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="17.375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -5264,7 +5306,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>98</v>
       </c>
@@ -5298,12 +5340,12 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -5311,7 +5353,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -5342,17 +5384,17 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" customWidth="1"/>
-    <col min="8" max="8" width="53.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.125" customWidth="1"/>
+    <col min="2" max="2" width="23.875" customWidth="1"/>
+    <col min="3" max="3" width="22.625" customWidth="1"/>
+    <col min="4" max="4" width="24.125" customWidth="1"/>
+    <col min="5" max="5" width="23.875" customWidth="1"/>
+    <col min="8" max="8" width="53.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -5375,7 +5417,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>99</v>
       </c>
@@ -5398,22 +5440,22 @@
         <v>44014</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G8" s="5"/>
     </row>
   </sheetData>

</xml_diff>